<commit_message>
Updated the test suite with final test results, Fixed a bug with the efficiency slider
</commit_message>
<xml_diff>
--- a/testing/test suite.xlsx
+++ b/testing/test suite.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gregr\Desktop\school\Semester 6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gregr\PycharmProjects\Space-Apps-AC23\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171FCC14-5079-4B6F-BD59-F28C81388D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E674516-97E2-4364-88E4-CFC751E888F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F9331D84-CCEE-4372-AEAB-E8DD9F5DA0CB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="231">
   <si>
     <t>Test Case</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Feature</t>
-  </si>
-  <si>
-    <t>FRONT END</t>
   </si>
   <si>
     <t>Loading Screen</t>
@@ -967,6 +964,354 @@
 Pygame window in place of the data 
 visualizer, further testing will be provided
 for the vizualizer module)</t>
+  </si>
+  <si>
+    <t>Apply filters from each category (name
+mass, distance) to refine
+the planet selection list</t>
+  </si>
+  <si>
+    <t>starting from original test data set of planets.
+1)Submit name = "er"
+2)submit distance = "100"
+3)submit mass = "600"</t>
+  </si>
+  <si>
+    <t>1) 5 results containing er found "Mercury, Jupiter, Hermes, 1a Mercury
+     ,5e Juipter"
+2) 2 results found "Mercury, Jupiter"
+3) 1 result found "Jupiter"</t>
+  </si>
+  <si>
+    <t>PASS - applying a secondary filter of a different category further filters 
+the existing filtered list by the secondary filter value</t>
+  </si>
+  <si>
+    <t>Apply multiple name filters in succession</t>
+  </si>
+  <si>
+    <t>starting from original test data set of planets.
+1)Submit name = "er"
+2)submit name = "M"
+3)submit name = "mercury"</t>
+  </si>
+  <si>
+    <t>1) 5 results containing er found "Mercury, Jupiter, Hermes, 1a Mercury
+     ,5e Juipter"
+2) 3 results found "Mercury, Hermes, 1a Mercury"
+3) 2 result found "Mercury, 1a Mercury"</t>
+  </si>
+  <si>
+    <t>PASS - Applying multiple filters of the same category further refines the 
+existing filtered list by each value entered.</t>
+  </si>
+  <si>
+    <t>Apply multiple Range filters in succession</t>
+  </si>
+  <si>
+    <t>starting from original test data set of planets.
+1)Submit range = "1000"
+2)submit range = "100"
+3)submit range = "25"</t>
+  </si>
+  <si>
+    <t>Apply multiple distance filters in succession</t>
+  </si>
+  <si>
+    <t>starting from original test data set of planets.
+1)Submit mass = "26000"
+2)submit mass = "1000"
+3)submit mass = "50"</t>
+  </si>
+  <si>
+    <t>1) 24 results found " all planets except unique "
+2) 10 results found
+3) 2 results found " Mars, Jupiter"</t>
+  </si>
+  <si>
+    <t>1) 24 results found " all planets except unique "
+2) 14 results found
+3) 2 results found " Cronus, 5 e Juipter"</t>
+  </si>
+  <si>
+    <t>Applying multiple filters resulting in a 
+selected planet list with a  population of
+0</t>
+  </si>
+  <si>
+    <t>starting from original test data set of planets.
+1)Submit name = "earth"
+2)submit mass = "100"
+3)submit mass = "5"</t>
+  </si>
+  <si>
+    <t>No results found.
+Selection list is automatially set to "No results found"</t>
+  </si>
+  <si>
+    <t>PASS - applying multiple filters until the filtered planet list becomes a population of 0 results in the selection list and select value being set to "No results found"</t>
+  </si>
+  <si>
+    <t>selecting a planet from the drop down list
+clicking calculate launches a top-level
+pygame window.
+The pygame window displays the correct
+model data for the selected planet.
+"Name, range, mass, efficiency index"</t>
+  </si>
+  <si>
+    <t>Select "Earth" from the available planet list.
+Set efficiency index to a value other then 1.
+(10)
+Click claculate.</t>
+  </si>
+  <si>
+    <t>A top level pygame window is launched.
+The window prints the appropriate values for "earth" 
+planet name = Earth
+Distance from Earth = 75.4392 pc
+Mass = 1525.5 Earth Masses
+calculation Efficiency Index = 10</t>
+  </si>
+  <si>
+    <t>PASS - Selecting an available planet and clicking calculate Launches 
+a top level pygame window with the appropriate model values of the
+selected planet to be passed to the algorithm.</t>
+  </si>
+  <si>
+    <t>Clicking calculate when the select value is
+"Select a planet"</t>
+  </si>
+  <si>
+    <t>Clear filters to ensure the Selection value is
+set to "select a planet".
+Click calculate.</t>
+  </si>
+  <si>
+    <t>No action is taken, and the selection value remains the same.
+A pygame window is not launched and a console MSG = "Invalid 
+selectiopn, please choose a planet from drop down!"</t>
+  </si>
+  <si>
+    <t>PASS - Clicking claculate when the selection value is invalid results in
+no action taken and an appropriate console MSG = "Invalid 
+selectiopn, please choose a planet from drop down!"</t>
+  </si>
+  <si>
+    <t>clicking Ccalculate when the select value is
+"No results found"</t>
+  </si>
+  <si>
+    <t>submit "xxx" in name filter to refine list to
+a 0 population result.
+Click claculate.</t>
+  </si>
+  <si>
+    <t>No action is taken, and the selection value remains the same.
+A pygame window is not launched and a console MSG = "No results
+containing "xxx" found"</t>
+  </si>
+  <si>
+    <t>PASS - Clicking claculate when the selection value is invalid results in
+no action taken and an appropriate console MSG = "No results
+containing "xxx" found"</t>
+  </si>
+  <si>
+    <t>ALGORITHM AND VISUALIZATION</t>
+  </si>
+  <si>
+    <t>Algorithmic results only appear after the
+visualization animation has completed. The algorithm results are appended to the planet
+information window on the left of the screen. The distance to the edge of the universe appears to the right of the selected planet sprite.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select "earth" from drop down list.
+Click claculate.
+Observe results after animation has
+completed. </t>
+  </si>
+  <si>
+    <t>Algorithmic results text appears in the planet information text
+box following the completion of the animation.
+Distance to edge of universe appears to the right of the selected
+planet sprite following the completion of the animation.</t>
+  </si>
+  <si>
+    <t>PASS - Calculation results appear after the animation has completed.</t>
+  </si>
+  <si>
+    <t>ALGORITHM ( some test results are 
+approximate values due to system 
+specifications affecting values like time
+taken to complete )</t>
+  </si>
+  <si>
+    <t>test algorithmic results at efficiency index
+of 1</t>
+  </si>
+  <si>
+    <t>test algorithmic results at efficiency index
+of 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select "earth" from drop down list.
+Set efficiency index to 1 or default.
+Click calculate.
+Observe results after animation has
+completed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">select "earth" from drop down list.
+Set efficiency index to 100.
+Click claculate.
+Observe results after animation has
+completed. </t>
+  </si>
+  <si>
+    <t>Planet name = "earth"
+Efficiency index = 1
+Expansion Time = 4.178e+37 years
+apprx Calculation time = 1 second
+Number of calculation = 200,000
+Intial Velocity = 0.0053 km/s
+Distance to edge of universe = 46.508 billion light years</t>
+  </si>
+  <si>
+    <t>PASS - 
+Planet name = "earth"
+Efficiency index = 1
+Expansion Time = 4.178e+37 years
+Calculation time = 0.0731 seconds
+Number of calculation = 200,000
+Intial Velocity = 0.0053 km/s
+Distance to edge of universe = 46.508 billion light years</t>
+  </si>
+  <si>
+    <t>Planet name = "earth"
+Efficiency index = 100
+Expansion Time = 4.178e+35 years
+apprx Calculation time = 4-6 seconds
+Number of calculation = 20,00,000
+Intial Velocity = 0.0053 km/s
+Distance to edge of universe = 46.508 billion light years</t>
+  </si>
+  <si>
+    <t>PASS - 
+Planet name = "earth"
+Efficiency index = 100
+Expansion Time = 4.178e+35 years
+apprx Calculation time = 4-6 seconds
+Number of calculation = 20,00,000
+Intial Velocity = 0.0053 km/s
+Distance to edge of universe = 46.508 billion light years</t>
+  </si>
+  <si>
+    <t>Test system stability at efficiency index
+of 1 for the MIN and MAX intial distance
+values available in production data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submit efficiency index of 1 or default.
+1) select "Proxima Cen b" click calculate.
+2) select "SWEEPS-4 b" click calculate.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALGORITHM LIMIT TESTS ( all tests 
+performed using the Largest and
+smallest distance data available in the 
+production data set)
+MIN Distance:
+Proxima Cen b = 1.30119
+MAX distance:
+SWEEPS-4 b
+</t>
+  </si>
+  <si>
+    <t>Algorithm performs calculations without overflow or underflow.
+1)
+Planet name = "Proxima Ceb b"
+Efficiency index = 1
+Expansion Time = 2.4223e+39 years
+apprx Calculation time = 1 seconds
+Number of calculation = 200,000
+Intial Velocity = 0.0001 km/s
+Distance to edge of universe = 46.508 billion light years
+2)
+Planet name = "SWEEPS-4 b"
+Efficiency index = 1
+Expansion Time = 3.7081e+35 years
+apprx Calculation time = 1 seconds
+Number of calculation = 200,000
+Intial Velocity = 0.5933 km/s
+Distance to edge of universe = 46.508 billion light years</t>
+  </si>
+  <si>
+    <t>PASS - The system does not crash at efficiency index of 1 when applied to the MIN and MAX available limits.
+1)
+Planet name = "Proxima Ceb b"
+Efficiency index = 1
+Expansion Time = 2.4223e+39 years
+apprx Calculation time = 1 seconds
+Number of calculation = 200,000
+Intial Velocity = 0.0001 km/s
+Distance to edge of universe = 46.508 billion light years
+2)
+Planet name = "SWEEPS-4 b"
+Efficiency index = 1
+Expansion Time = 3.7081e+35 years
+apprx Calculation time = 1 seconds
+Number of calculation = 200,000
+Intial Velocity = 0.5933 km/s
+Distance to edge of universe = 46.508 billion light years</t>
+  </si>
+  <si>
+    <t>Submit efficiency index of 100.
+1) select "Proxima Cen b" click calculate.
+2) select "SWEEPS-4 b" click calculate.</t>
+  </si>
+  <si>
+    <t>Test system stability at efficiency index
+of 100 for the MIN and MAX intial distance
+values available in production data.</t>
+  </si>
+  <si>
+    <t>Algorithm performs calculations without overflow or underflow.
+1)
+Planet name = "Proxima Ceb b"
+Efficiency index = 100
+Expansion Time = 2.4223e+37 years
+apprx Calculation time = 6.1221 seconds
+Number of calculation = 2,000,000
+Intial Velocity = 0.0001 km/s
+Distance to edge of universe = 46.508 billion light years
+2)
+Planet name = "SWEEPS-4 b"
+Efficiency index = 100
+Expansion Time = 3.7081e+33 years
+apprx Calculation time = 5-6 seconds
+Number of calculation = 2,000,000
+Intial Velocity = 0.5933 km/s
+Distance to edge of universe = 46.508 billion light years</t>
+  </si>
+  <si>
+    <t>PASS - The system does not crash at efficiency index of 100 when applied to the MIN and MAX available limits.
+1)
+Planet name = "Proxima Ceb b"
+Efficiency index = 100
+Expansion Time = 2.4223e+37 years
+apprx Calculation time = 6.1221 seconds
+Number of calculation = 2,000,000
+Intial Velocity = 0.0001 km/s
+Distance to edge of universe = 46.508 billion light years
+2)
+Planet name = "SWEEPS-4 b"
+Efficiency index = 100
+Expansion Time = 3.7081e+33 years
+apprx Calculation time = 5-6 seconds
+Number of calculation = 2,000,000
+Intial Velocity = 0.5933 km/s
+Distance to edge of universe = 46.508 billion light years</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1149,88 +1494,100 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1547,803 +1904,986 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C0D75A-8F95-40F9-9F5C-A3CB6F784262}">
-  <dimension ref="A2:H55"/>
+  <dimension ref="A2:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="40" style="6" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="64.140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="40" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="62.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="64.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="11" t="s">
+      <c r="D14" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="B28" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="F29" s="27"/>
+    </row>
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="B30" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F30" s="27"/>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="F31" s="27"/>
+    </row>
+    <row r="32" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="B32" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="F32" s="27"/>
+    </row>
+    <row r="33" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="B33" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="F33" s="27"/>
+    </row>
+    <row r="34" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="18"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+    </row>
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="B42" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+    </row>
+    <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="B46" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E46" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+    </row>
+    <row r="48" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A49" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E49" s="23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+      <c r="A50" s="11"/>
+      <c r="B50" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="E50" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" ht="240" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="180" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="E27" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="C28" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="C29" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="E29" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="F29" s="30"/>
-    </row>
-    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="F30" s="30"/>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="E31" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="F31" s="30"/>
-    </row>
-    <row r="32" spans="1:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="F32" s="30"/>
-    </row>
-    <row r="33" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="F33" s="30"/>
-    </row>
-    <row r="34" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
+      <c r="F50" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A51" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+      <c r="A52" s="11"/>
+      <c r="B52" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="E52" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D53" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A54" s="11"/>
+      <c r="B54" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A55" s="11"/>
+      <c r="B55" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A56" s="11"/>
+      <c r="B56" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="E56" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="11"/>
+      <c r="B57" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="11"/>
+      <c r="B58" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="E58" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A59" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-    </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C37" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E37" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="E39" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-    </row>
-    <row r="41" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B41" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C41" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="E41" s="19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C42" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="E42" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-    </row>
-    <row r="44" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="B44" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="E44" s="19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A45" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C45" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="D45" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E45" s="26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="225" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="C46" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="D46" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="E46" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="F46" s="13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="B47" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="C47" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="D47" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E47" s="19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="240" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="D48" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="E48" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F48" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="B49" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D49" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="E49" s="22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="C50" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="D50" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="E50" s="26" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="C51" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="D51" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="C52" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="D52" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="E52" s="26" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="C53" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="D53" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
-      <c r="B54" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="C54" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="D54" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="E54" s="26" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A55" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
+      <c r="B59" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="E59" s="16" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E60" s="31" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B61" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E61" s="32" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="34" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A64" s="35" t="s">
+        <v>213</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E64" s="33" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B65" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E65" s="32" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B66" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E66" s="31" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="300" x14ac:dyDescent="0.25">
+      <c r="A67" s="35" t="s">
+        <v>224</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E67" s="31" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="300" x14ac:dyDescent="0.25">
+      <c r="B68" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E68" s="32" t="s">
+        <v>230</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>